<commit_message>
modeleJury mis a jour
</commit_message>
<xml_diff>
--- a/src/images/ModeleS1Jury.xlsx
+++ b/src/images/ModeleS1Jury.xlsx
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t xml:space="preserve">BUT 1  INFORMATIQUE</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t xml:space="preserve">BUT 2 INFORMATIQUE</t>
   </si>
   <si>
     <t xml:space="preserve">SEMESTRE 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 - 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JURY DU 14 MARS 2024</t>
   </si>
   <si>
     <t xml:space="preserve">code_nip</t>
@@ -230,7 +224,7 @@
   <dimension ref="A2:T90"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -269,9 +263,7 @@
     </row>
     <row r="4" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F4" s="1"/>
-      <c r="G4" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -280,9 +272,7 @@
     </row>
     <row r="5" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F5" s="1"/>
-      <c r="G5" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -292,64 +282,64 @@
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="P8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="Q8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="R8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="S8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="T8" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>